<commit_message>
First components order by David
</commit_message>
<xml_diff>
--- a/Documents/Datalogging Finances.xlsx
+++ b/Documents/Datalogging Finances.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="9885" windowHeight="5895" activeTab="1"/>
+    <workbookView xWindow="7660" yWindow="140" windowWidth="14940" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -313,7 +318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +347,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,15 +391,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -391,8 +420,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,23 +729,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G348"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32:J37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="9" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -736,7 +768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="6">
         <v>41577</v>
       </c>
@@ -760,7 +792,7 @@
         <v>82.76</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="6">
         <v>41577</v>
       </c>
@@ -784,7 +816,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="6">
         <v>41577</v>
       </c>
@@ -808,7 +840,7 @@
         <v>9.69</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="6">
         <v>41577</v>
       </c>
@@ -832,7 +864,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="6">
         <v>41577</v>
       </c>
@@ -856,7 +888,7 @@
         <v>12.21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="6">
         <v>41579</v>
       </c>
@@ -880,7 +912,7 @@
         <v>3.3000000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="6">
         <v>41579</v>
       </c>
@@ -904,7 +936,7 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="6">
         <v>41579</v>
       </c>
@@ -928,7 +960,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="6">
         <v>41579</v>
       </c>
@@ -952,7 +984,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="6">
         <v>41579</v>
       </c>
@@ -976,7 +1008,7 @@
         <v>1.7399999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="6">
         <v>41579</v>
       </c>
@@ -1000,7 +1032,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="6">
         <v>41579</v>
       </c>
@@ -1024,7 +1056,7 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="6">
         <v>41579</v>
       </c>
@@ -1048,7 +1080,7 @@
         <v>5.66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="6">
         <v>41590</v>
       </c>
@@ -1072,7 +1104,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="6">
         <v>41599</v>
       </c>
@@ -1096,7 +1128,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="6">
         <v>41599</v>
       </c>
@@ -1120,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="6">
         <v>41603</v>
       </c>
@@ -1144,7 +1176,7 @@
         <v>4.0599999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="6">
         <v>41615</v>
       </c>
@@ -1168,7 +1200,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="6">
         <v>41615</v>
       </c>
@@ -1192,7 +1224,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="6">
         <v>41615</v>
       </c>
@@ -1216,7 +1248,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="6">
         <v>41615</v>
       </c>
@@ -1240,7 +1272,7 @@
         <v>6.46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="6">
         <v>41615</v>
       </c>
@@ -1264,7 +1296,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="6">
         <v>41660</v>
       </c>
@@ -1288,7 +1320,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="6">
         <v>41660</v>
       </c>
@@ -1312,7 +1344,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="6">
         <v>41660</v>
       </c>
@@ -1336,7 +1368,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="6">
         <v>41660</v>
       </c>
@@ -1360,7 +1392,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="6">
         <v>41669</v>
       </c>
@@ -1384,7 +1416,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="6">
         <v>41673</v>
       </c>
@@ -1408,7 +1440,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="6">
         <v>41673</v>
       </c>
@@ -1432,7 +1464,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="6">
         <v>41673</v>
       </c>
@@ -1456,7 +1488,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="6">
         <v>41673</v>
       </c>
@@ -1480,7 +1512,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="6">
         <v>41673</v>
       </c>
@@ -1504,7 +1536,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="6">
         <v>41673</v>
       </c>
@@ -1528,7 +1560,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="6">
         <v>41673</v>
       </c>
@@ -1552,7 +1584,7 @@
         <v>1.7199999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="6">
         <v>41673</v>
       </c>
@@ -1576,7 +1608,7 @@
         <v>2.3499999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="6">
         <v>41673</v>
       </c>
@@ -1600,7 +1632,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="6">
         <v>41673</v>
       </c>
@@ -1624,7 +1656,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="6">
         <v>41673</v>
       </c>
@@ -1648,7 +1680,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="6">
         <v>41673</v>
       </c>
@@ -1672,7 +1704,7 @@
         <v>10.91</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="6">
         <v>41694</v>
       </c>
@@ -1696,7 +1728,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="6">
         <v>41699</v>
       </c>
@@ -1720,7 +1752,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="6">
         <v>41703</v>
       </c>
@@ -1744,7 +1776,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="6">
         <v>41703</v>
       </c>
@@ -1768,7 +1800,7 @@
         <v>9.69</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="6">
         <v>41703</v>
       </c>
@@ -1792,7 +1824,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="6">
         <v>41703</v>
       </c>
@@ -1816,7 +1848,7 @@
         <v>0.33600000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="6">
         <v>41703</v>
       </c>
@@ -1840,7 +1872,7 @@
         <v>8.14</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="6">
         <v>41703</v>
       </c>
@@ -1864,7 +1896,7 @@
         <v>1.6900000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="6">
         <v>41703</v>
       </c>
@@ -1888,1803 +1920,1940 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
+      <c r="A50" s="6">
+        <v>41767</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="12">
+        <v>2342641</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="3">
+        <v>6.46</v>
+      </c>
+      <c r="F50" s="4">
+        <v>1</v>
+      </c>
       <c r="G50" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="6">
+        <f>A50</f>
+        <v>41767</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="12">
+        <v>8650101</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="F51" s="4">
+        <v>10</v>
+      </c>
       <c r="G51" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="6">
+        <f t="shared" ref="A52:A59" si="2">A51</f>
+        <v>41767</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1017687</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="F52" s="4">
+        <v>10</v>
+      </c>
       <c r="G52" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="12">
+        <v>2310212</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="F53" s="4">
+        <v>2</v>
+      </c>
       <c r="G53" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="12">
+        <v>2293708</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1.69</v>
+      </c>
+      <c r="F54" s="4">
+        <v>2</v>
+      </c>
       <c r="G54" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="12">
+        <v>9589899</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="F55" s="4">
+        <v>3</v>
+      </c>
       <c r="G55" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="F56" s="4">
+        <v>20</v>
+      </c>
       <c r="G56" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="G57" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="G58" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="G59" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="G60" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="G61" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="G62" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="G63" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="G64" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:7">
       <c r="G65" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:7">
       <c r="G66" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:7">
       <c r="G67" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:7">
       <c r="G68" s="3">
-        <f t="shared" ref="G68:G131" si="2">E68*F68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G68:G131" si="3">E68*F68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7">
       <c r="G69" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7">
       <c r="G70" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7">
       <c r="G71" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7">
       <c r="G72" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7">
       <c r="G73" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7">
       <c r="G74" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7">
       <c r="G75" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7">
       <c r="G76" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7">
       <c r="G77" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7">
       <c r="G78" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7">
       <c r="G79" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7">
       <c r="G80" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7">
       <c r="G81" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7">
       <c r="G82" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7">
       <c r="G83" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7">
       <c r="G84" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7">
       <c r="G85" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7">
       <c r="G86" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7">
       <c r="G87" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7">
       <c r="G88" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7">
       <c r="G89" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7">
       <c r="G90" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7">
       <c r="G91" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7">
       <c r="G92" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7">
       <c r="G93" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7">
       <c r="G94" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7">
       <c r="G95" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7">
       <c r="G96" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7">
       <c r="G97" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7">
       <c r="G98" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7">
       <c r="G99" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7">
       <c r="G100" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7">
       <c r="G101" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7">
       <c r="G102" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7">
       <c r="G103" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7">
       <c r="G104" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7">
       <c r="G105" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7">
       <c r="G106" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7">
       <c r="G107" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7">
       <c r="G108" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7">
       <c r="G109" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7">
       <c r="G110" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7">
       <c r="G111" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7">
       <c r="G112" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7">
       <c r="G113" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7">
       <c r="G114" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7">
       <c r="G115" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7">
       <c r="G116" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7">
       <c r="G117" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="7:7">
       <c r="G118" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="7:7">
       <c r="G119" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="7:7">
       <c r="G120" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="7:7">
       <c r="G121" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="7:7">
       <c r="G122" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7">
       <c r="G123" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="7:7">
       <c r="G124" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="7:7">
       <c r="G125" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="7:7">
       <c r="G126" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="7:7">
       <c r="G127" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="7:7">
       <c r="G128" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="7:7">
       <c r="G129" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="7:7">
       <c r="G130" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7">
       <c r="G131" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="7:7">
       <c r="G132" s="3">
-        <f t="shared" ref="G132:G195" si="3">E132*F132</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G132:G195" si="4">E132*F132</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="7:7">
       <c r="G133" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="7:7">
       <c r="G134" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="7:7">
       <c r="G135" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="7:7">
       <c r="G136" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="7:7">
       <c r="G137" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="7:7">
       <c r="G138" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="7:7">
       <c r="G139" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="7:7">
       <c r="G140" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="7:7">
       <c r="G141" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="7:7">
       <c r="G142" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="7:7">
       <c r="G143" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="7:7">
       <c r="G144" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="7:7">
       <c r="G145" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="7:7">
       <c r="G146" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="7:7">
       <c r="G147" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="7:7">
       <c r="G148" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="7:7">
       <c r="G149" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="7:7">
       <c r="G150" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="7:7">
       <c r="G151" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="7:7">
       <c r="G152" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="7:7">
       <c r="G153" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="7:7">
       <c r="G154" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7">
       <c r="G155" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="7:7">
       <c r="G156" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="7:7">
       <c r="G157" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="7:7">
       <c r="G158" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="7:7">
       <c r="G159" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="7:7">
       <c r="G160" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="7:7">
       <c r="G161" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="7:7">
       <c r="G162" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="7:7">
       <c r="G163" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="7:7">
       <c r="G164" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="7:7">
       <c r="G165" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="7:7">
       <c r="G166" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="7:7">
       <c r="G167" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="7:7">
       <c r="G168" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="7:7">
       <c r="G169" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="7:7">
       <c r="G170" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="7:7">
       <c r="G171" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="7:7">
       <c r="G172" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="7:7">
       <c r="G173" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="7:7">
       <c r="G174" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="7:7">
       <c r="G175" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="7:7">
       <c r="G176" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="7:7">
       <c r="G177" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="7:7">
       <c r="G178" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="7:7">
       <c r="G179" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="7:7">
       <c r="G180" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="7:7">
       <c r="G181" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="7:7">
       <c r="G182" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="7:7">
       <c r="G183" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="7:7">
       <c r="G184" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="7:7">
       <c r="G185" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="7:7">
       <c r="G186" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="7:7">
       <c r="G187" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="7:7">
       <c r="G188" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="7:7">
       <c r="G189" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="7:7">
       <c r="G190" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="7:7">
       <c r="G191" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="7:7">
       <c r="G192" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="7:7">
       <c r="G193" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="7:7">
       <c r="G194" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="7:7">
       <c r="G195" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="7:7">
       <c r="G196" s="3">
-        <f t="shared" ref="G196:G259" si="4">E196*F196</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G196:G259" si="5">E196*F196</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="7:7">
       <c r="G197" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="7:7">
       <c r="G198" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="7:7">
       <c r="G199" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="7:7">
       <c r="G200" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="7:7">
       <c r="G201" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="7:7">
       <c r="G202" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="7:7">
       <c r="G203" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="7:7">
       <c r="G204" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="7:7">
       <c r="G205" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="7:7">
       <c r="G206" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="7:7">
       <c r="G207" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="7:7">
       <c r="G208" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="7:7">
       <c r="G209" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="7:7">
       <c r="G210" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="7:7">
       <c r="G211" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="7:7">
       <c r="G212" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="7:7">
       <c r="G213" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="7:7">
       <c r="G214" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="7:7">
       <c r="G215" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="7:7">
       <c r="G216" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="7:7">
       <c r="G217" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="7:7">
       <c r="G218" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="7:7">
       <c r="G219" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="7:7">
       <c r="G220" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7">
       <c r="G221" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="7:7">
       <c r="G222" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="7:7">
       <c r="G223" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="7:7">
       <c r="G224" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="7:7">
       <c r="G225" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7">
       <c r="G226" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="7:7">
       <c r="G227" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7">
       <c r="G228" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="7:7">
       <c r="G229" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7">
       <c r="G230" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="7:7">
       <c r="G231" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7">
       <c r="G232" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="7:7">
       <c r="G233" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7">
       <c r="G234" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="7:7">
       <c r="G235" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="7:7">
       <c r="G236" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="7:7">
       <c r="G237" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="7:7">
       <c r="G238" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="7:7">
       <c r="G239" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="7:7">
       <c r="G240" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="7:7">
       <c r="G241" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="7:7">
       <c r="G242" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="7:7">
       <c r="G243" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="7:7">
       <c r="G244" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="7:7">
       <c r="G245" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="7:7">
       <c r="G246" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="7:7">
       <c r="G247" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="7:7">
       <c r="G248" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="7:7">
       <c r="G249" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="7:7">
       <c r="G250" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="7:7">
       <c r="G251" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="7:7">
       <c r="G252" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="7:7">
       <c r="G253" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="7:7">
       <c r="G254" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="7:7">
       <c r="G255" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="7:7">
       <c r="G256" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="7:7">
       <c r="G257" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="7:7">
       <c r="G258" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="7:7">
       <c r="G259" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="7:7">
       <c r="G260" s="3">
-        <f t="shared" ref="G260:G323" si="5">E260*F260</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G260:G323" si="6">E260*F260</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="7:7">
       <c r="G261" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="7:7">
       <c r="G262" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="7:7">
       <c r="G263" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="7:7">
       <c r="G264" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="7:7">
       <c r="G265" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="7:7">
       <c r="G266" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="7:7">
       <c r="G267" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="7:7">
       <c r="G268" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="7:7">
       <c r="G269" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="7:7">
       <c r="G270" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="7:7">
       <c r="G271" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="7:7">
       <c r="G272" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="7:7">
       <c r="G273" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="7:7">
       <c r="G274" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="7:7">
       <c r="G275" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="7:7">
       <c r="G276" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="7:7">
       <c r="G277" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="7:7">
       <c r="G278" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="7:7">
       <c r="G279" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="7:7">
       <c r="G280" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="7:7">
       <c r="G281" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="7:7">
       <c r="G282" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="7:7">
       <c r="G283" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="7:7">
       <c r="G284" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="7:7">
       <c r="G285" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="7:7">
       <c r="G286" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="7:7">
       <c r="G287" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="7:7">
       <c r="G288" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="7:7">
       <c r="G289" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="7:7">
       <c r="G290" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="7:7">
       <c r="G291" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="7:7">
       <c r="G292" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="7:7">
       <c r="G293" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="7:7">
       <c r="G294" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="7:7">
       <c r="G295" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="7:7">
       <c r="G296" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="7:7">
       <c r="G297" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="7:7">
       <c r="G298" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="7:7">
       <c r="G299" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="7:7">
       <c r="G300" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="7:7">
       <c r="G301" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="7:7">
       <c r="G302" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="7:7">
       <c r="G303" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="7:7">
       <c r="G304" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="7:7">
       <c r="G305" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="306" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="7:7">
       <c r="G306" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="7:7">
       <c r="G307" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="7:7">
       <c r="G308" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="7:7">
       <c r="G309" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="7:7">
       <c r="G310" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="7:7">
       <c r="G311" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="7:7">
       <c r="G312" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="7:7">
       <c r="G313" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="7:7">
       <c r="G314" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="7:7">
       <c r="G315" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="7:7">
       <c r="G316" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="7:7">
       <c r="G317" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="7:7">
       <c r="G318" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="7:7">
       <c r="G319" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="7:7">
       <c r="G320" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="7:7">
       <c r="G321" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="7:7">
       <c r="G322" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="7:7">
       <c r="G323" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="7:7">
       <c r="G324" s="3">
-        <f t="shared" ref="G324:G348" si="6">E324*F324</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G324:G348" si="7">E324*F324</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="7:7">
       <c r="G325" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="7:7">
       <c r="G326" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="327" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="7:7">
       <c r="G327" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="328" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="7:7">
       <c r="G328" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="329" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="7:7">
       <c r="G329" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="330" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="7:7">
       <c r="G330" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="331" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="7:7">
       <c r="G331" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="332" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="7:7">
       <c r="G332" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="333" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="7:7">
       <c r="G333" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="334" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="7:7">
       <c r="G334" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="335" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="7:7">
       <c r="G335" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="336" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="7:7">
       <c r="G336" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="337" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="7:7">
       <c r="G337" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="338" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="7:7">
       <c r="G338" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="339" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="7:7">
       <c r="G339" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="340" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="7:7">
       <c r="G340" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="341" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="7:7">
       <c r="G341" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="342" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="7:7">
       <c r="G342" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="343" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="7:7">
       <c r="G343" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="344" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="7:7">
       <c r="G344" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="345" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="7:7">
       <c r="G345" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="346" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="7:7">
       <c r="G346" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="7:7">
       <c r="G347" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="348" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="7:7">
       <c r="G348" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3692,19 +3861,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
@@ -3718,7 +3887,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -3739,7 +3908,7 @@
         <v>92.158999999999992</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>77</v>
       </c>
@@ -3757,7 +3926,7 @@
         <v>23.234000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -3775,7 +3944,7 @@
         <v>19.724</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -3793,7 +3962,7 @@
         <v>13.843999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>56</v>
       </c>
@@ -3811,7 +3980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -3822,7 +3991,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -3833,7 +4002,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -3844,7 +4013,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>63</v>
       </c>
@@ -3855,7 +4024,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>65</v>
       </c>
@@ -3866,7 +4035,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>64</v>
       </c>
@@ -3877,7 +4046,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>66</v>
       </c>
@@ -3888,7 +4057,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>67</v>
       </c>
@@ -3899,7 +4068,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>68</v>
       </c>
@@ -3910,7 +4079,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -3921,7 +4090,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -3932,7 +4101,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" t="s">
         <v>62</v>
       </c>
@@ -3943,7 +4112,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -3954,7 +4123,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -3965,7 +4134,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -3976,7 +4145,7 @@
         <v>42.21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" t="s">
         <v>71</v>
       </c>
@@ -3984,7 +4153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" t="s">
         <v>72</v>
       </c>
@@ -3992,7 +4161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" t="s">
         <v>73</v>
       </c>
@@ -4000,7 +4169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="B25" t="s">
         <v>75</v>
       </c>
@@ -4011,7 +4180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -4025,7 +4194,7 @@
         <v>13.48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" t="s">
         <v>81</v>
       </c>
@@ -4036,7 +4205,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" t="s">
         <v>82</v>
       </c>
@@ -4047,7 +4216,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="B30" t="s">
         <v>66</v>
       </c>
@@ -4058,7 +4227,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" t="s">
         <v>67</v>
       </c>
@@ -4069,7 +4238,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" t="s">
         <v>68</v>
       </c>
@@ -4080,7 +4249,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="B33" t="s">
         <v>63</v>
       </c>
@@ -4091,7 +4260,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="B34" t="s">
         <v>65</v>
       </c>
@@ -4102,7 +4271,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="B35" t="s">
         <v>64</v>
       </c>
@@ -4113,7 +4282,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="B36" t="s">
         <v>85</v>
       </c>
@@ -4124,7 +4293,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -4138,7 +4307,7 @@
         <v>12.92</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="B39" t="s">
         <v>82</v>
       </c>
@@ -4149,7 +4318,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="B40" t="s">
         <v>66</v>
       </c>
@@ -4160,7 +4329,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="B41" t="s">
         <v>67</v>
       </c>
@@ -4171,7 +4340,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="B42" t="s">
         <v>68</v>
       </c>
@@ -4182,7 +4351,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="B43" t="s">
         <v>63</v>
       </c>
@@ -4193,7 +4362,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="B44" t="s">
         <v>65</v>
       </c>
@@ -4204,7 +4373,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="B45" t="s">
         <v>64</v>
       </c>
@@ -4215,7 +4384,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="B46" t="s">
         <v>85</v>
       </c>
@@ -4226,7 +4395,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -4234,7 +4403,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="B49" t="s">
         <v>87</v>
       </c>
@@ -4245,7 +4414,7 @@
         <v>5.66</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="B50" t="s">
         <v>82</v>
       </c>
@@ -4256,7 +4425,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="B51" t="s">
         <v>88</v>
       </c>
@@ -4267,7 +4436,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="B52" t="s">
         <v>66</v>
       </c>
@@ -4278,7 +4447,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="B53" t="s">
         <v>67</v>
       </c>
@@ -4289,7 +4458,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="B54" t="s">
         <v>68</v>
       </c>
@@ -4300,7 +4469,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="B55" t="s">
         <v>63</v>
       </c>
@@ -4311,7 +4480,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="B56" t="s">
         <v>65</v>
       </c>
@@ -4322,7 +4491,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="B57" t="s">
         <v>64</v>
       </c>
@@ -4333,7 +4502,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="B58" t="s">
         <v>85</v>
       </c>
@@ -4344,7 +4513,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -4358,7 +4527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="B61" t="s">
         <v>91</v>
       </c>
@@ -4369,7 +4538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="B62" t="s">
         <v>92</v>
       </c>
@@ -4382,7 +4551,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4390,10 +4564,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A38" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DC Current Board - Done by Saurab
</commit_message>
<xml_diff>
--- a/Documents/Datalogging Finances.xlsx
+++ b/Documents/Datalogging Finances.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="9885" windowHeight="5895" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="9885" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>AC Board Toal Cost</t>
+  </si>
+  <si>
+    <t>ABS Box 353x140x122</t>
   </si>
 </sst>
 </file>
@@ -697,9 +700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G348"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32:J37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,15 +1892,51 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>41764</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="F50" s="4">
+        <v>2</v>
+      </c>
       <c r="G50" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>41764</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="9">
+        <v>1526660</v>
+      </c>
+      <c r="D51" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="3">
+        <v>11.32</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
       <c r="G51" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.32</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3692,7 +3731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v1.0, AC sinewave algorithm
</commit_message>
<xml_diff>
--- a/Documents/Datalogging Finances.xlsx
+++ b/Documents/Datalogging Finances.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="9885" windowHeight="5895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -306,17 +311,51 @@
     <t>AC Board Toal Cost</t>
   </si>
   <si>
-    <t>ABS Box 353x140x122</t>
+    <t>PRO POWER - PV516A GROMMET PK 100 - GROMMET, BLANK, 31.8MM, PK100</t>
+  </si>
+  <si>
+    <t>MULTICOMP - KTSC-22R - CAP, ROUND, RED</t>
+  </si>
+  <si>
+    <t>MULTICOMP - KTSC-22K - CAP, ROUND, BLACK, 13MM</t>
+  </si>
+  <si>
+    <t>DURATOOL - M4- HFA2-S100- - FULL NUT, STAINLESS STEEL, A2, M4</t>
+  </si>
+  <si>
+    <t>ETTINGER - 05.03.143 - SPACER, M3X14-NI</t>
+  </si>
+  <si>
+    <t>VISHAY - TLLG4401 - LED, 3MM, GREEN, 2MCD, 565NM</t>
+  </si>
+  <si>
+    <t>VISHAY - TLLR4401 - LED, 3MM, HE-RED</t>
+  </si>
+  <si>
+    <t>MULTICOMP - LED3-4 - LED HOLDER, ROUND, 3MM, 2 PIN</t>
+  </si>
+  <si>
+    <t>BOURNS - 3386F-1-101LF - TRIMMER, 100R</t>
+  </si>
+  <si>
+    <t>TE CONNECTIVITY / AMP - 0-0881545-2 - JUMPER, WITH HANDLE, 2.54MM, 2WAY</t>
+  </si>
+  <si>
+    <t>PRO POWER - PVC TAPE 1920B - TAPE, BLACK, 19MMX20M</t>
+  </si>
+  <si>
+    <t>MULTICOMP - 2212S-20SG-85 - SOCKET, PCB, 1 ROW, 20WAY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +384,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -367,15 +433,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -394,8 +462,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -700,23 +773,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G348"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="9" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -739,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="6">
         <v>41577</v>
       </c>
@@ -763,7 +836,7 @@
         <v>82.76</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="6">
         <v>41577</v>
       </c>
@@ -787,7 +860,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="6">
         <v>41577</v>
       </c>
@@ -811,7 +884,7 @@
         <v>9.69</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="6">
         <v>41577</v>
       </c>
@@ -835,7 +908,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="6">
         <v>41577</v>
       </c>
@@ -859,7 +932,7 @@
         <v>12.21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="6">
         <v>41579</v>
       </c>
@@ -883,7 +956,7 @@
         <v>3.3000000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="6">
         <v>41579</v>
       </c>
@@ -907,7 +980,7 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="6">
         <v>41579</v>
       </c>
@@ -931,7 +1004,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="6">
         <v>41579</v>
       </c>
@@ -955,7 +1028,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="6">
         <v>41579</v>
       </c>
@@ -979,7 +1052,7 @@
         <v>1.7399999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="6">
         <v>41579</v>
       </c>
@@ -1003,7 +1076,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="6">
         <v>41579</v>
       </c>
@@ -1027,7 +1100,7 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="6">
         <v>41579</v>
       </c>
@@ -1051,7 +1124,7 @@
         <v>5.66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="6">
         <v>41590</v>
       </c>
@@ -1075,7 +1148,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="6">
         <v>41599</v>
       </c>
@@ -1099,7 +1172,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="6">
         <v>41599</v>
       </c>
@@ -1123,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="6">
         <v>41603</v>
       </c>
@@ -1147,7 +1220,7 @@
         <v>4.0599999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="6">
         <v>41615</v>
       </c>
@@ -1171,7 +1244,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="6">
         <v>41615</v>
       </c>
@@ -1195,7 +1268,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="6">
         <v>41615</v>
       </c>
@@ -1219,7 +1292,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="6">
         <v>41615</v>
       </c>
@@ -1243,7 +1316,7 @@
         <v>6.46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="6">
         <v>41615</v>
       </c>
@@ -1267,7 +1340,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="6">
         <v>41660</v>
       </c>
@@ -1291,7 +1364,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="6">
         <v>41660</v>
       </c>
@@ -1315,7 +1388,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="6">
         <v>41660</v>
       </c>
@@ -1339,7 +1412,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="6">
         <v>41660</v>
       </c>
@@ -1363,7 +1436,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="6">
         <v>41669</v>
       </c>
@@ -1387,7 +1460,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="6">
         <v>41673</v>
       </c>
@@ -1411,7 +1484,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="6">
         <v>41673</v>
       </c>
@@ -1435,7 +1508,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="6">
         <v>41673</v>
       </c>
@@ -1459,7 +1532,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="6">
         <v>41673</v>
       </c>
@@ -1483,7 +1556,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="6">
         <v>41673</v>
       </c>
@@ -1507,7 +1580,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="6">
         <v>41673</v>
       </c>
@@ -1531,7 +1604,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="6">
         <v>41673</v>
       </c>
@@ -1555,7 +1628,7 @@
         <v>1.7199999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="6">
         <v>41673</v>
       </c>
@@ -1579,7 +1652,7 @@
         <v>2.3499999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="6">
         <v>41673</v>
       </c>
@@ -1603,7 +1676,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="6">
         <v>41673</v>
       </c>
@@ -1627,7 +1700,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="6">
         <v>41673</v>
       </c>
@@ -1651,7 +1724,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="6">
         <v>41673</v>
       </c>
@@ -1675,7 +1748,7 @@
         <v>10.91</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="6">
         <v>41694</v>
       </c>
@@ -1699,7 +1772,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="6">
         <v>41699</v>
       </c>
@@ -1723,7 +1796,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="6">
         <v>41703</v>
       </c>
@@ -1747,7 +1820,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="6">
         <v>41703</v>
       </c>
@@ -1771,7 +1844,7 @@
         <v>9.69</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="6">
         <v>41703</v>
       </c>
@@ -1795,7 +1868,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="6">
         <v>41703</v>
       </c>
@@ -1819,7 +1892,7 @@
         <v>0.33600000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="6">
         <v>41703</v>
       </c>
@@ -1843,7 +1916,7 @@
         <v>8.14</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="6">
         <v>41703</v>
       </c>
@@ -1867,7 +1940,7 @@
         <v>1.6900000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="6">
         <v>41703</v>
       </c>
@@ -1891,1839 +1964,2167 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="6">
-        <v>41764</v>
+        <v>41767</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" t="s">
-        <v>51</v>
+        <v>7</v>
+      </c>
+      <c r="C50" s="12">
+        <v>2342641</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="E50" s="3">
-        <v>0.58499999999999996</v>
+        <v>6.46</v>
       </c>
       <c r="F50" s="4">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="0"/>
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="6">
+        <f>A50</f>
+        <v>41767</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="12">
+        <v>8650101</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="F51" s="4">
+        <v>10</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" si="0"/>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="6">
+        <f t="shared" ref="A52:A56" si="2">A51</f>
+        <v>41767</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1017687</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="F52" s="4">
+        <v>10</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="12">
+        <v>2310212</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="F53" s="4">
         <v>2</v>
       </c>
-      <c r="G50" s="3">
-        <f t="shared" si="0"/>
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
-        <v>41764</v>
-      </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="9">
-        <v>1526660</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="G53" s="3">
+        <f t="shared" si="0"/>
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="12">
+        <v>2293708</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1.69</v>
+      </c>
+      <c r="F54" s="4">
+        <v>2</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="0"/>
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="12">
+        <v>9589899</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="F55" s="4">
+        <v>3</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="6">
+        <f t="shared" si="2"/>
+        <v>41767</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="F56" s="4">
+        <v>20</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="6">
+        <v>41771</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="13">
+        <v>1189053</v>
+      </c>
+      <c r="D57" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="3">
-        <v>11.32</v>
-      </c>
-      <c r="F51" s="4">
+      <c r="E57" s="14">
+        <v>10.58</v>
+      </c>
+      <c r="F57" s="13">
         <v>1</v>
       </c>
-      <c r="G51" s="3">
-        <f t="shared" si="0"/>
-        <v>11.32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G52" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G53" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G56" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G57" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="6">
+        <f>A57</f>
+        <v>41771</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="13">
+        <v>9561536</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="F58" s="13">
+        <v>10</v>
+      </c>
       <c r="G58" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="6">
+        <f t="shared" ref="A59:A68" si="3">A58</f>
+        <v>41771</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="13">
+        <v>9561552</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F59" s="13">
+        <v>10</v>
+      </c>
       <c r="G59" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="13">
+        <v>1420790</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E60" s="14">
+        <v>3.37</v>
+      </c>
+      <c r="F60" s="13">
+        <v>1</v>
+      </c>
       <c r="G60" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="13">
+        <v>1466812</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F61" s="13">
+        <v>25</v>
+      </c>
       <c r="G61" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="13">
+        <v>1045505</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="14">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F62" s="13">
+        <v>10</v>
+      </c>
       <c r="G62" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="13">
+        <v>1045504</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E63" s="14">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="F63" s="13">
+        <v>5</v>
+      </c>
       <c r="G63" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="13">
+        <v>9555242</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" s="13">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F64" s="13">
+        <v>25</v>
+      </c>
       <c r="G64" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="13">
+        <v>9354522</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="F65" s="13">
+        <v>3</v>
+      </c>
       <c r="G65" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="13">
+        <v>4218176</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" s="14">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F66" s="13">
+        <v>10</v>
+      </c>
       <c r="G66" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+        <v>1.3900000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="13">
+        <v>152346</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E67" s="14">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F67" s="13">
+        <v>2</v>
+      </c>
       <c r="G67" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="6">
+        <f t="shared" si="3"/>
+        <v>41771</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="13">
+        <v>1593469</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" s="14">
+        <v>1.23</v>
+      </c>
+      <c r="F68" s="13">
+        <v>5</v>
+      </c>
       <c r="G68" s="3">
-        <f t="shared" ref="G68:G131" si="2">E68*F68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G68:G131" si="4">E68*F68</f>
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="G69" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="G70" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="G71" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="G72" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="G73" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="G74" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="G75" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="G76" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="G77" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="G78" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="G79" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="G80" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7">
       <c r="G81" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7">
       <c r="G82" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7">
       <c r="G83" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7">
       <c r="G84" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7">
       <c r="G85" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7">
       <c r="G86" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7">
       <c r="G87" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7">
       <c r="G88" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7">
       <c r="G89" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7">
       <c r="G90" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7">
       <c r="G91" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7">
       <c r="G92" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7">
       <c r="G93" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7">
       <c r="G94" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7">
       <c r="G95" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7">
       <c r="G96" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7">
       <c r="G97" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7">
       <c r="G98" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7">
       <c r="G99" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7">
       <c r="G100" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7">
       <c r="G101" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7">
       <c r="G102" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7">
       <c r="G103" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7">
       <c r="G104" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7">
       <c r="G105" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7">
       <c r="G106" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7">
       <c r="G107" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7">
       <c r="G108" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7">
       <c r="G109" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7">
       <c r="G110" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7">
       <c r="G111" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7">
       <c r="G112" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7">
       <c r="G113" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7">
       <c r="G114" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7">
       <c r="G115" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7">
       <c r="G116" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7">
       <c r="G117" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="7:7">
       <c r="G118" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="7:7">
       <c r="G119" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="7:7">
       <c r="G120" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="7:7">
       <c r="G121" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="7:7">
       <c r="G122" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7">
       <c r="G123" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="7:7">
       <c r="G124" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="7:7">
       <c r="G125" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="7:7">
       <c r="G126" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="7:7">
       <c r="G127" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="7:7">
       <c r="G128" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="7:7">
       <c r="G129" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="7:7">
       <c r="G130" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="7:7">
       <c r="G131" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="7:7">
       <c r="G132" s="3">
-        <f t="shared" ref="G132:G195" si="3">E132*F132</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G132:G195" si="5">E132*F132</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="7:7">
       <c r="G133" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="7:7">
       <c r="G134" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="7:7">
       <c r="G135" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="7:7">
       <c r="G136" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="7:7">
       <c r="G137" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="7:7">
       <c r="G138" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="7:7">
       <c r="G139" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="7:7">
       <c r="G140" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="7:7">
       <c r="G141" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="7:7">
       <c r="G142" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="7:7">
       <c r="G143" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="7:7">
       <c r="G144" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="7:7">
       <c r="G145" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="7:7">
       <c r="G146" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="7:7">
       <c r="G147" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="7:7">
       <c r="G148" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="7:7">
       <c r="G149" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="7:7">
       <c r="G150" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="7:7">
       <c r="G151" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="7:7">
       <c r="G152" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="7:7">
       <c r="G153" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="7:7">
       <c r="G154" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7">
       <c r="G155" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="7:7">
       <c r="G156" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="7:7">
       <c r="G157" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="7:7">
       <c r="G158" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="7:7">
       <c r="G159" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="7:7">
       <c r="G160" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="7:7">
       <c r="G161" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="7:7">
       <c r="G162" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="7:7">
       <c r="G163" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="7:7">
       <c r="G164" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="7:7">
       <c r="G165" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="7:7">
       <c r="G166" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="7:7">
       <c r="G167" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="7:7">
       <c r="G168" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="7:7">
       <c r="G169" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="7:7">
       <c r="G170" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="7:7">
       <c r="G171" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="7:7">
       <c r="G172" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="7:7">
       <c r="G173" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="7:7">
       <c r="G174" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="7:7">
       <c r="G175" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="7:7">
       <c r="G176" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="7:7">
       <c r="G177" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="7:7">
       <c r="G178" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="7:7">
       <c r="G179" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="7:7">
       <c r="G180" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="7:7">
       <c r="G181" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="7:7">
       <c r="G182" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="7:7">
       <c r="G183" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="7:7">
       <c r="G184" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="7:7">
       <c r="G185" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="7:7">
       <c r="G186" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="7:7">
       <c r="G187" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="7:7">
       <c r="G188" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="7:7">
       <c r="G189" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="7:7">
       <c r="G190" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="7:7">
       <c r="G191" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="7:7">
       <c r="G192" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="7:7">
       <c r="G193" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="7:7">
       <c r="G194" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="7:7">
       <c r="G195" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="7:7">
       <c r="G196" s="3">
-        <f t="shared" ref="G196:G259" si="4">E196*F196</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G196:G259" si="6">E196*F196</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="7:7">
       <c r="G197" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="7:7">
       <c r="G198" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="7:7">
       <c r="G199" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="7:7">
       <c r="G200" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="7:7">
       <c r="G201" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="7:7">
       <c r="G202" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="7:7">
       <c r="G203" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="7:7">
       <c r="G204" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="7:7">
       <c r="G205" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="7:7">
       <c r="G206" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="7:7">
       <c r="G207" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="7:7">
       <c r="G208" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="7:7">
       <c r="G209" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="7:7">
       <c r="G210" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="7:7">
       <c r="G211" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="7:7">
       <c r="G212" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="7:7">
       <c r="G213" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="7:7">
       <c r="G214" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="7:7">
       <c r="G215" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="7:7">
       <c r="G216" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="7:7">
       <c r="G217" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="7:7">
       <c r="G218" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="7:7">
       <c r="G219" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="7:7">
       <c r="G220" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7">
       <c r="G221" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="7:7">
       <c r="G222" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="7:7">
       <c r="G223" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="7:7">
       <c r="G224" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="7:7">
       <c r="G225" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7">
       <c r="G226" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="7:7">
       <c r="G227" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7">
       <c r="G228" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="7:7">
       <c r="G229" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7">
       <c r="G230" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="7:7">
       <c r="G231" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7">
       <c r="G232" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="7:7">
       <c r="G233" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7">
       <c r="G234" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="7:7">
       <c r="G235" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="7:7">
       <c r="G236" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="7:7">
       <c r="G237" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="7:7">
       <c r="G238" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="7:7">
       <c r="G239" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="7:7">
       <c r="G240" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="7:7">
       <c r="G241" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="7:7">
       <c r="G242" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="7:7">
       <c r="G243" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="7:7">
       <c r="G244" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="7:7">
       <c r="G245" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="7:7">
       <c r="G246" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="7:7">
       <c r="G247" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="7:7">
       <c r="G248" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="7:7">
       <c r="G249" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="7:7">
       <c r="G250" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="7:7">
       <c r="G251" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="7:7">
       <c r="G252" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="7:7">
       <c r="G253" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="7:7">
       <c r="G254" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="7:7">
       <c r="G255" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="7:7">
       <c r="G256" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="7:7">
       <c r="G257" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="7:7">
       <c r="G258" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="7:7">
       <c r="G259" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="7:7">
       <c r="G260" s="3">
-        <f t="shared" ref="G260:G323" si="5">E260*F260</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G260:G323" si="7">E260*F260</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="7:7">
       <c r="G261" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="7:7">
       <c r="G262" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="7:7">
       <c r="G263" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="7:7">
       <c r="G264" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="7:7">
       <c r="G265" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="7:7">
       <c r="G266" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="7:7">
       <c r="G267" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="7:7">
       <c r="G268" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="7:7">
       <c r="G269" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="7:7">
       <c r="G270" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="7:7">
       <c r="G271" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="7:7">
       <c r="G272" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="7:7">
       <c r="G273" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="7:7">
       <c r="G274" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="7:7">
       <c r="G275" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="7:7">
       <c r="G276" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="7:7">
       <c r="G277" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="7:7">
       <c r="G278" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="7:7">
       <c r="G279" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="7:7">
       <c r="G280" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="7:7">
       <c r="G281" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="7:7">
       <c r="G282" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="7:7">
       <c r="G283" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="7:7">
       <c r="G284" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="7:7">
       <c r="G285" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="7:7">
       <c r="G286" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="7:7">
       <c r="G287" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="7:7">
       <c r="G288" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="7:7">
       <c r="G289" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="7:7">
       <c r="G290" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="7:7">
       <c r="G291" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="7:7">
       <c r="G292" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="7:7">
       <c r="G293" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="7:7">
       <c r="G294" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="7:7">
       <c r="G295" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="7:7">
       <c r="G296" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="7:7">
       <c r="G297" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="7:7">
       <c r="G298" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="7:7">
       <c r="G299" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="7:7">
       <c r="G300" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="7:7">
       <c r="G301" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="7:7">
       <c r="G302" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="7:7">
       <c r="G303" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="7:7">
       <c r="G304" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="305" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="7:7">
       <c r="G305" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="306" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="7:7">
       <c r="G306" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="307" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="7:7">
       <c r="G307" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="7:7">
       <c r="G308" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="7:7">
       <c r="G309" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="7:7">
       <c r="G310" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="7:7">
       <c r="G311" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="7:7">
       <c r="G312" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="313" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="7:7">
       <c r="G313" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="7:7">
       <c r="G314" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="7:7">
       <c r="G315" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="7:7">
       <c r="G316" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="7:7">
       <c r="G317" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="7:7">
       <c r="G318" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="7:7">
       <c r="G319" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="7:7">
       <c r="G320" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="7:7">
       <c r="G321" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="7:7">
       <c r="G322" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="7:7">
       <c r="G323" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="7:7">
       <c r="G324" s="3">
-        <f t="shared" ref="G324:G348" si="6">E324*F324</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G324:G348" si="8">E324*F324</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="7:7">
       <c r="G325" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="7:7">
       <c r="G326" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="327" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="7:7">
       <c r="G327" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="328" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="7:7">
       <c r="G328" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="329" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="7:7">
       <c r="G329" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="330" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="7:7">
       <c r="G330" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="331" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="7:7">
       <c r="G331" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="332" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="7:7">
       <c r="G332" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="333" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="7:7">
       <c r="G333" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="334" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="7:7">
       <c r="G334" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="335" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="7:7">
       <c r="G335" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="336" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="7:7">
       <c r="G336" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="337" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="7:7">
       <c r="G337" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="338" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="7:7">
       <c r="G338" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="339" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="7:7">
       <c r="G339" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="340" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="7:7">
       <c r="G340" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="341" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="7:7">
       <c r="G341" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="342" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="7:7">
       <c r="G342" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="343" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="7:7">
       <c r="G343" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="344" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="7:7">
       <c r="G344" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="345" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="7:7">
       <c r="G345" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="346" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="7:7">
       <c r="G346" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="7:7">
       <c r="G347" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="348" spans="7:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="7:7">
       <c r="G348" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3731,19 +4132,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
@@ -3757,7 +4158,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -3778,7 +4179,7 @@
         <v>92.158999999999992</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>77</v>
       </c>
@@ -3796,7 +4197,7 @@
         <v>23.234000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -3814,7 +4215,7 @@
         <v>19.724</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -3832,7 +4233,7 @@
         <v>13.843999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>56</v>
       </c>
@@ -3850,7 +4251,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -3861,7 +4262,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -3872,7 +4273,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -3883,7 +4284,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>63</v>
       </c>
@@ -3894,7 +4295,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>65</v>
       </c>
@@ -3905,7 +4306,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>64</v>
       </c>
@@ -3916,7 +4317,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>66</v>
       </c>
@@ -3927,7 +4328,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>67</v>
       </c>
@@ -3938,7 +4339,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>68</v>
       </c>
@@ -3949,7 +4350,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -3960,7 +4361,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -3971,7 +4372,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" t="s">
         <v>62</v>
       </c>
@@ -3982,7 +4383,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -3993,7 +4394,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -4004,7 +4405,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -4015,7 +4416,7 @@
         <v>42.21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" t="s">
         <v>71</v>
       </c>
@@ -4023,7 +4424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" t="s">
         <v>72</v>
       </c>
@@ -4031,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" t="s">
         <v>73</v>
       </c>
@@ -4039,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="B25" t="s">
         <v>75</v>
       </c>
@@ -4050,7 +4451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -4064,7 +4465,7 @@
         <v>13.48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="B28" t="s">
         <v>81</v>
       </c>
@@ -4075,7 +4476,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="B29" t="s">
         <v>82</v>
       </c>
@@ -4086,7 +4487,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="B30" t="s">
         <v>66</v>
       </c>
@@ -4097,7 +4498,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="B31" t="s">
         <v>67</v>
       </c>
@@ -4108,7 +4509,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="B32" t="s">
         <v>68</v>
       </c>
@@ -4119,7 +4520,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="B33" t="s">
         <v>63</v>
       </c>
@@ -4130,7 +4531,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="B34" t="s">
         <v>65</v>
       </c>
@@ -4141,7 +4542,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="B35" t="s">
         <v>64</v>
       </c>
@@ -4152,7 +4553,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="B36" t="s">
         <v>85</v>
       </c>
@@ -4163,7 +4564,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -4177,7 +4578,7 @@
         <v>12.92</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="B39" t="s">
         <v>82</v>
       </c>
@@ -4188,7 +4589,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="B40" t="s">
         <v>66</v>
       </c>
@@ -4199,7 +4600,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="B41" t="s">
         <v>67</v>
       </c>
@@ -4210,7 +4611,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="B42" t="s">
         <v>68</v>
       </c>
@@ -4221,7 +4622,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="B43" t="s">
         <v>63</v>
       </c>
@@ -4232,7 +4633,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="B44" t="s">
         <v>65</v>
       </c>
@@ -4243,7 +4644,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="B45" t="s">
         <v>64</v>
       </c>
@@ -4254,7 +4655,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="B46" t="s">
         <v>85</v>
       </c>
@@ -4265,7 +4666,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -4273,7 +4674,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="B49" t="s">
         <v>87</v>
       </c>
@@ -4284,7 +4685,7 @@
         <v>5.66</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="B50" t="s">
         <v>82</v>
       </c>
@@ -4295,7 +4696,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="B51" t="s">
         <v>88</v>
       </c>
@@ -4306,7 +4707,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="B52" t="s">
         <v>66</v>
       </c>
@@ -4317,7 +4718,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="B53" t="s">
         <v>67</v>
       </c>
@@ -4328,7 +4729,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="B54" t="s">
         <v>68</v>
       </c>
@@ -4339,7 +4740,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="B55" t="s">
         <v>63</v>
       </c>
@@ -4350,7 +4751,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="B56" t="s">
         <v>65</v>
       </c>
@@ -4361,7 +4762,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="B57" t="s">
         <v>64</v>
       </c>
@@ -4372,7 +4773,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="B58" t="s">
         <v>85</v>
       </c>
@@ -4383,7 +4784,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -4397,7 +4798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="B61" t="s">
         <v>91</v>
       </c>
@@ -4408,7 +4809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="B62" t="s">
         <v>92</v>
       </c>
@@ -4421,7 +4822,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4429,10 +4835,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A38" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>